<commit_message>
gng WF add STD
</commit_message>
<xml_diff>
--- a/R01_riskstatus.xlsx
+++ b/R01_riskstatus.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24617"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365.sharepoint.com/sites/b-childfoodlab/Shared Documents/Box Migration Data/b-childfoodlab_Shared/Active_Studies/RO1_Brain_Mechanisms_IRB_5357/Participant_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{3D158407-978A-B846-8CAA-6E37C8341D39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{AA79F67C-B25D-714D-A06E-8890E9E9E8C3}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{3D158407-978A-B846-8CAA-6E37C8341D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{455DFD23-5B76-4665-BE66-E571A0C3B70D}"/>
   <bookViews>
     <workbookView xWindow="2360" yWindow="500" windowWidth="27640" windowHeight="16440" xr2:uid="{86014519-78CF-114E-A40D-0D49A70F3C8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="4">
   <si>
     <t>ID</t>
   </si>
@@ -38,17 +42,17 @@
     <t>Risk</t>
   </si>
   <si>
-    <t>Low</t>
+    <t>High</t>
   </si>
   <si>
-    <t>High</t>
+    <t>Low</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,15 +397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C0B5CA-3111-2045-8B62-0B7A9AD0CD4A}">
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,664 +413,672 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12">
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13">
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14">
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15">
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16">
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52">
         <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54">
         <v>80</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55">
         <v>81</v>
       </c>
       <c r="B55" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56">
         <v>82</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57">
         <v>83</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58">
         <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59">
         <v>89</v>
       </c>
       <c r="B59" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60">
         <v>90</v>
       </c>
       <c r="B60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61">
         <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62">
         <v>94</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63">
         <v>95</v>
       </c>
       <c r="B63" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64">
         <v>96</v>
       </c>
       <c r="B64" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65">
         <v>98</v>
       </c>
       <c r="B65" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66">
         <v>101</v>
       </c>
       <c r="B66" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67">
         <v>103</v>
       </c>
       <c r="B67" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68">
         <v>104</v>
       </c>
       <c r="B68" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69">
         <v>105</v>
       </c>
       <c r="B69" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70">
         <v>106</v>
       </c>
       <c r="B70" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71">
         <v>107</v>
       </c>
       <c r="B71" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72">
         <v>109</v>
       </c>
       <c r="B72" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73">
         <v>111</v>
       </c>
       <c r="B73" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74">
         <v>112</v>
       </c>
       <c r="B74" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75">
         <v>113</v>
       </c>
       <c r="B75" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76">
         <v>115</v>
       </c>
       <c r="B76" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77">
         <v>116</v>
       </c>
       <c r="B77" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78">
         <v>117</v>
       </c>
       <c r="B78" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79">
         <v>118</v>
       </c>
       <c r="B79" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80">
         <v>119</v>
       </c>
       <c r="B80" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81">
         <v>120</v>
       </c>
       <c r="B81" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82">
         <v>121</v>
       </c>
       <c r="B82" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83">
         <v>122</v>
       </c>
       <c r="B83" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84">
+        <v>123</v>
+      </c>
+      <c r="B84" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B83">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B83">
     <sortCondition ref="A2:A83"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1074,6 +1086,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000FF1B0174AE16E4CB1CC41FAEDE75A33" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="054cdb9d99f894db796ababf7b791478">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6" xmlns:ns3="cf6faeb8-54d1-4580-a175-bd3097eaab2a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c10d8bc434365a681a376bfc5a38d7dd" ns2:_="" ns3:_="">
     <xsd:import namespace="2c4f76d2-e5fd-4d0c-9f1c-02c6c8d48dd6"/>
@@ -1290,15 +1311,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1306,11 +1318,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1146BE9D-AB01-4CF8-A10F-69575D79C13F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D0F72BE-6F53-412A-9E60-CA043307454A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D0F72BE-6F53-412A-9E60-CA043307454A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1146BE9D-AB01-4CF8-A10F-69575D79C13F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>